<commit_message>
5.3.2. Data Preparation Finished not discussed yet
</commit_message>
<xml_diff>
--- a/google_analytics_schema.xlsx
+++ b/google_analytics_schema.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="711">
   <si>
     <t>visitorId</t>
   </si>
@@ -2122,9 +2122,6 @@
     <t>product_quantity</t>
   </si>
   <si>
-    <t>social_source_referral</t>
-  </si>
-  <si>
     <t>client_id</t>
   </si>
   <si>
@@ -2174,6 +2171,51 @@
   </si>
   <si>
     <t>Variable Name</t>
+  </si>
+  <si>
+    <t>referral_path</t>
+  </si>
+  <si>
+    <t>campaign</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>ad_content</t>
+  </si>
+  <si>
+    <t>ad_page</t>
+  </si>
+  <si>
+    <t>ad_slot</t>
+  </si>
+  <si>
+    <t>page_keyword</t>
+  </si>
+  <si>
+    <t>traffic_keyword</t>
+  </si>
+  <si>
+    <t>social_action</t>
+  </si>
+  <si>
+    <t>social_interactions</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>is_social_referral</t>
+  </si>
+  <si>
+    <t>social_interaction_network</t>
+  </si>
+  <si>
+    <t>network_action</t>
+  </si>
+  <si>
+    <t>unique_social_interactions</t>
   </si>
 </sst>
 </file>
@@ -2260,8 +2302,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tbValidFields" displayName="tbValidFields" ref="A1:L126" totalsRowShown="0">
-  <autoFilter ref="A1:L126"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tbValidFields" displayName="tbValidFields" ref="A1:L131" totalsRowShown="0">
+  <autoFilter ref="A1:L131">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="trafficSource.adContent"/>
+        <filter val="trafficSource.adwordsClickInfo.adNetworkType"/>
+        <filter val="trafficSource.adwordsClickInfo.gclId"/>
+        <filter val="trafficSource.adwordsClickInfo.isVideoAd"/>
+        <filter val="trafficSource.adwordsClickInfo.page"/>
+        <filter val="trafficSource.adwordsClickInfo.slot"/>
+        <filter val="trafficSource.campaign"/>
+        <filter val="trafficSource.campaignCode"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="6" name="#"/>
     <tableColumn id="1" name="Field Name"/>
@@ -2545,8 +2600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C258"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A76" sqref="A71:A76"/>
+    <sheetView topLeftCell="A214" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A221" sqref="A221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5410,10 +5465,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L126"/>
+  <dimension ref="A1:L131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5438,7 +5493,7 @@
         <v>257</v>
       </c>
       <c r="C1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D1" t="s">
         <v>633</v>
@@ -5468,7 +5523,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5488,7 +5543,7 @@
         <v>646</v>
       </c>
       <c r="G2" t="s">
-        <v>653</v>
+        <v>640</v>
       </c>
       <c r="H2" t="s">
         <v>1</v>
@@ -5506,7 +5561,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5523,7 +5578,7 @@
         <v>637</v>
       </c>
       <c r="F3" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="G3" t="s">
         <v>653</v>
@@ -5544,7 +5599,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5579,7 +5634,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5617,7 +5672,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5655,7 +5710,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5690,7 +5745,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5707,7 +5762,7 @@
         <v>638</v>
       </c>
       <c r="F8" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="G8" t="s">
         <v>640</v>
@@ -5728,7 +5783,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5766,7 +5821,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5801,7 +5856,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5818,7 +5873,7 @@
         <v>638</v>
       </c>
       <c r="F11" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="G11" t="s">
         <v>640</v>
@@ -5839,7 +5894,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5874,7 +5929,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5909,7 +5964,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5944,7 +5999,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="72" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5979,13 +6034,16 @@
         <v>535</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
       </c>
+      <c r="C16" t="s">
+        <v>696</v>
+      </c>
       <c r="D16" t="s">
         <v>635</v>
       </c>
@@ -5993,7 +6051,7 @@
         <v>643</v>
       </c>
       <c r="F16" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G16" t="s">
         <v>641</v>
@@ -6021,6 +6079,9 @@
       <c r="B17" t="s">
         <v>23</v>
       </c>
+      <c r="C17" t="s">
+        <v>697</v>
+      </c>
       <c r="D17" t="s">
         <v>635</v>
       </c>
@@ -6028,7 +6089,7 @@
         <v>638</v>
       </c>
       <c r="F17" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G17" t="s">
         <v>641</v>
@@ -6049,13 +6110,16 @@
         <v>546</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
       </c>
+      <c r="C18" t="s">
+        <v>698</v>
+      </c>
       <c r="D18" t="s">
         <v>635</v>
       </c>
@@ -6063,7 +6127,7 @@
         <v>643</v>
       </c>
       <c r="F18" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="G18" t="s">
         <v>641</v>
@@ -6084,7 +6148,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6122,13 +6186,16 @@
         <v>548</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
       </c>
+      <c r="C20" t="s">
+        <v>703</v>
+      </c>
       <c r="D20" t="s">
         <v>635</v>
       </c>
@@ -6136,7 +6203,7 @@
         <v>643</v>
       </c>
       <c r="F20" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="G20" t="s">
         <v>641</v>
@@ -6164,6 +6231,9 @@
       <c r="B21" t="s">
         <v>27</v>
       </c>
+      <c r="C21" t="s">
+        <v>699</v>
+      </c>
       <c r="D21" t="s">
         <v>635</v>
       </c>
@@ -6171,7 +6241,7 @@
         <v>638</v>
       </c>
       <c r="F21" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="G21" t="s">
         <v>641</v>
@@ -6199,6 +6269,9 @@
       <c r="B22" t="s">
         <v>33</v>
       </c>
+      <c r="C22" t="s">
+        <v>700</v>
+      </c>
       <c r="D22" t="s">
         <v>635</v>
       </c>
@@ -6206,7 +6279,7 @@
         <v>638</v>
       </c>
       <c r="F22" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G22" t="s">
         <v>641</v>
@@ -6234,6 +6307,9 @@
       <c r="B23" t="s">
         <v>34</v>
       </c>
+      <c r="C23" t="s">
+        <v>701</v>
+      </c>
       <c r="D23" t="s">
         <v>635</v>
       </c>
@@ -6241,7 +6317,7 @@
         <v>638</v>
       </c>
       <c r="F23" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="G23" t="s">
         <v>641</v>
@@ -6367,7 +6443,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -6375,7 +6451,7 @@
         <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D27" t="s">
         <v>635</v>
@@ -6437,7 +6513,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6475,7 +6551,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6513,7 +6589,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6548,7 +6624,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6586,7 +6662,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6624,7 +6700,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -6662,7 +6738,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -6670,7 +6746,7 @@
         <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D35" t="s">
         <v>635</v>
@@ -6700,7 +6776,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -6708,7 +6784,7 @@
         <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D36" t="s">
         <v>635</v>
@@ -6738,7 +6814,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6746,7 +6822,7 @@
         <v>68</v>
       </c>
       <c r="C37" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D37" t="s">
         <v>635</v>
@@ -6776,7 +6852,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -6814,7 +6890,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6822,7 +6898,7 @@
         <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D39" t="s">
         <v>635</v>
@@ -6852,7 +6928,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6884,7 +6960,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -6922,7 +6998,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -6957,7 +7033,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -6992,7 +7068,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -7030,7 +7106,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -7065,7 +7141,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -7100,7 +7176,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -7135,7 +7211,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -7167,7 +7243,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -7175,7 +7251,7 @@
         <v>89</v>
       </c>
       <c r="C49" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D49" t="s">
         <v>635</v>
@@ -7205,7 +7281,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -7240,7 +7316,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -7275,13 +7351,16 @@
         <v>576</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>92</v>
       </c>
+      <c r="C52" t="s">
+        <v>702</v>
+      </c>
       <c r="D52" t="s">
         <v>635</v>
       </c>
@@ -7289,7 +7368,7 @@
         <v>638</v>
       </c>
       <c r="F52" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G52" t="s">
         <v>641</v>
@@ -7310,7 +7389,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -7345,7 +7424,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -7353,7 +7432,7 @@
         <v>94</v>
       </c>
       <c r="C54" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D54" t="s">
         <v>635</v>
@@ -7383,7 +7462,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -7391,7 +7470,7 @@
         <v>95</v>
       </c>
       <c r="C55" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D55" t="s">
         <v>635</v>
@@ -7421,7 +7500,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -7429,7 +7508,7 @@
         <v>96</v>
       </c>
       <c r="C56" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D56" t="s">
         <v>635</v>
@@ -7459,7 +7538,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -7467,7 +7546,7 @@
         <v>97</v>
       </c>
       <c r="C57" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D57" t="s">
         <v>635</v>
@@ -7497,7 +7576,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -7535,7 +7614,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -7543,7 +7622,7 @@
         <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D59" t="s">
         <v>634</v>
@@ -7573,7 +7652,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -7608,7 +7687,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -7643,7 +7722,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -7678,7 +7757,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -7713,7 +7792,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -7748,7 +7827,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -7783,7 +7862,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -7818,7 +7897,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -7853,7 +7932,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -7888,7 +7967,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -7923,7 +8002,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -7958,7 +8037,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -7993,7 +8072,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -8028,7 +8107,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -8063,7 +8142,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -8098,7 +8177,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -8133,7 +8212,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -8171,7 +8250,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -8209,7 +8288,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -8247,7 +8326,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -8282,7 +8361,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -8320,7 +8399,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -8355,7 +8434,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -8390,7 +8469,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -8428,7 +8507,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -8463,7 +8542,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -8501,7 +8580,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -8536,7 +8615,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -8571,7 +8650,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -8606,7 +8685,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -8641,7 +8720,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -8676,7 +8755,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -8711,7 +8790,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -8746,7 +8825,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -8781,7 +8860,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -8816,7 +8895,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -8851,7 +8930,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="172.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" ht="172.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -8886,7 +8965,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -8921,7 +9000,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -8956,7 +9035,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" ht="57.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -8991,15 +9070,15 @@
         <v>611</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C100" t="s">
-        <v>669</v>
+        <v>707</v>
       </c>
       <c r="D100" t="s">
         <v>635</v>
@@ -9011,7 +9090,7 @@
         <v>646</v>
       </c>
       <c r="G100" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="H100" t="s">
         <v>6</v>
@@ -9020,24 +9099,21 @@
         <v>518</v>
       </c>
       <c r="J100">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="L100" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <v>100</v>
-      </c>
+        <v>613</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C101" t="s">
-        <v>679</v>
+        <v>704</v>
       </c>
       <c r="D101" t="s">
         <v>635</v>
@@ -9049,7 +9125,7 @@
         <v>646</v>
       </c>
       <c r="G101" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="H101" t="s">
         <v>6</v>
@@ -9057,22 +9133,19 @@
       <c r="I101" t="s">
         <v>518</v>
       </c>
-      <c r="J101">
-        <v>2</v>
-      </c>
-      <c r="K101" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="L101" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102">
-        <v>101</v>
-      </c>
+      <c r="J101" t="s">
+        <v>706</v>
+      </c>
+      <c r="K101" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
-        <v>230</v>
+        <v>221</v>
+      </c>
+      <c r="C102" t="s">
+        <v>708</v>
       </c>
       <c r="D102" t="s">
         <v>635</v>
@@ -9081,33 +9154,30 @@
         <v>638</v>
       </c>
       <c r="F102" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G102" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H102" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I102" t="s">
         <v>518</v>
       </c>
-      <c r="J102">
-        <v>368</v>
-      </c>
-      <c r="K102" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="L102" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103">
-        <v>102</v>
-      </c>
+      <c r="J102" t="s">
+        <v>706</v>
+      </c>
+      <c r="K102" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
-        <v>231</v>
+        <v>228</v>
+      </c>
+      <c r="C103" t="s">
+        <v>709</v>
       </c>
       <c r="D103" t="s">
         <v>635</v>
@@ -9116,33 +9186,30 @@
         <v>638</v>
       </c>
       <c r="F103" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G103" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H103" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I103" t="s">
         <v>518</v>
       </c>
-      <c r="J103">
-        <v>10606</v>
-      </c>
-      <c r="K103" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="L103" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104">
-        <v>103</v>
-      </c>
+      <c r="J103" t="s">
+        <v>706</v>
+      </c>
+      <c r="K103" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
-        <v>232</v>
+        <v>223</v>
+      </c>
+      <c r="C104" t="s">
+        <v>705</v>
       </c>
       <c r="D104" t="s">
         <v>635</v>
@@ -9151,7 +9218,7 @@
         <v>638</v>
       </c>
       <c r="F104" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G104" t="s">
         <v>640</v>
@@ -9162,22 +9229,19 @@
       <c r="I104" t="s">
         <v>518</v>
       </c>
-      <c r="J104">
-        <v>1764</v>
-      </c>
-      <c r="K104" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="L104" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105">
-        <v>104</v>
-      </c>
+      <c r="J104" t="s">
+        <v>706</v>
+      </c>
+      <c r="K104" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
-        <v>233</v>
+        <v>225</v>
+      </c>
+      <c r="C105" t="s">
+        <v>669</v>
       </c>
       <c r="D105" t="s">
         <v>635</v>
@@ -9186,33 +9250,33 @@
         <v>638</v>
       </c>
       <c r="F105" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G105" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H105" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I105" t="s">
         <v>518</v>
       </c>
       <c r="J105">
-        <v>2445</v>
+        <v>16</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>364</v>
+        <v>426</v>
       </c>
       <c r="L105" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106">
-        <v>105</v>
-      </c>
+        <v>612</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
-        <v>234</v>
+        <v>226</v>
+      </c>
+      <c r="C106" t="s">
+        <v>710</v>
       </c>
       <c r="D106" t="s">
         <v>635</v>
@@ -9221,7 +9285,7 @@
         <v>638</v>
       </c>
       <c r="F106" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G106" t="s">
         <v>640</v>
@@ -9232,22 +9296,19 @@
       <c r="I106" t="s">
         <v>518</v>
       </c>
-      <c r="J106">
-        <v>368</v>
-      </c>
-      <c r="K106" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="L106" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J106" t="s">
+        <v>706</v>
+      </c>
+      <c r="K106" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B107" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D107" t="s">
         <v>635</v>
@@ -9268,21 +9329,21 @@
         <v>518</v>
       </c>
       <c r="J107">
-        <v>1290</v>
+        <v>368</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="L107" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B108" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D108" t="s">
         <v>635</v>
@@ -9303,21 +9364,21 @@
         <v>518</v>
       </c>
       <c r="J108">
-        <v>1783</v>
+        <v>10606</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="L108" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B109" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D109" t="s">
         <v>635</v>
@@ -9338,21 +9399,21 @@
         <v>518</v>
       </c>
       <c r="J109">
-        <v>4473</v>
+        <v>1764</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L109" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B110" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D110" t="s">
         <v>635</v>
@@ -9373,21 +9434,21 @@
         <v>518</v>
       </c>
       <c r="J110">
-        <v>368</v>
+        <v>2445</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="L110" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B111" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D111" t="s">
         <v>635</v>
@@ -9408,21 +9469,21 @@
         <v>518</v>
       </c>
       <c r="J111">
-        <v>8339</v>
+        <v>368</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="L111" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B112" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D112" t="s">
         <v>635</v>
@@ -9443,62 +9504,56 @@
         <v>518</v>
       </c>
       <c r="J112">
-        <v>8383</v>
+        <v>1290</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L112" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B113" t="s">
-        <v>522</v>
-      </c>
-      <c r="C113" t="s">
-        <v>688</v>
+        <v>236</v>
       </c>
       <c r="D113" t="s">
         <v>635</v>
       </c>
       <c r="E113" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="F113" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="G113" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H113" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I113" t="s">
         <v>518</v>
       </c>
       <c r="J113">
-        <v>4</v>
+        <v>1783</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>649</v>
+        <v>365</v>
       </c>
       <c r="L113" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B114" t="s">
-        <v>524</v>
-      </c>
-      <c r="C114" t="s">
-        <v>690</v>
+        <v>237</v>
       </c>
       <c r="D114" t="s">
         <v>635</v>
@@ -9507,33 +9562,33 @@
         <v>638</v>
       </c>
       <c r="F114" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="G114" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H114" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I114" t="s">
         <v>518</v>
       </c>
       <c r="J114">
-        <v>10</v>
+        <v>4473</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>650</v>
+        <v>366</v>
       </c>
       <c r="L114" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B115" t="s">
-        <v>525</v>
+        <v>238</v>
       </c>
       <c r="D115" t="s">
         <v>635</v>
@@ -9545,68 +9600,65 @@
         <v>647</v>
       </c>
       <c r="G115" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H115" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I115" t="s">
         <v>518</v>
       </c>
       <c r="J115">
-        <v>3</v>
+        <v>368</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>651</v>
+        <v>360</v>
       </c>
       <c r="L115" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B116" t="s">
-        <v>526</v>
-      </c>
-      <c r="C116" t="s">
-        <v>689</v>
+        <v>239</v>
       </c>
       <c r="D116" t="s">
         <v>635</v>
       </c>
       <c r="E116" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="F116" t="s">
         <v>647</v>
       </c>
       <c r="G116" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H116" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I116" t="s">
         <v>518</v>
       </c>
       <c r="J116">
-        <v>5</v>
+        <v>8339</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>649</v>
+        <v>359</v>
       </c>
       <c r="L116" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B117" t="s">
-        <v>527</v>
+        <v>240</v>
       </c>
       <c r="D117" t="s">
         <v>635</v>
@@ -9618,39 +9670,42 @@
         <v>647</v>
       </c>
       <c r="G117" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H117" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I117" t="s">
         <v>518</v>
       </c>
       <c r="J117">
-        <v>11</v>
+        <v>8383</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>650</v>
+        <v>358</v>
       </c>
       <c r="L117" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B118" t="s">
-        <v>528</v>
+        <v>522</v>
+      </c>
+      <c r="C118" t="s">
+        <v>687</v>
       </c>
       <c r="D118" t="s">
         <v>635</v>
       </c>
       <c r="E118" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
       <c r="F118" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G118" t="s">
         <v>641</v>
@@ -9665,18 +9720,21 @@
         <v>4</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="L118" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B119" t="s">
-        <v>529</v>
+        <v>524</v>
+      </c>
+      <c r="C119" t="s">
+        <v>689</v>
       </c>
       <c r="D119" t="s">
         <v>635</v>
@@ -9685,7 +9743,7 @@
         <v>638</v>
       </c>
       <c r="F119" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G119" t="s">
         <v>641</v>
@@ -9697,21 +9755,21 @@
         <v>518</v>
       </c>
       <c r="J119">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>523</v>
+        <v>650</v>
       </c>
       <c r="L119" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B120" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="D120" t="s">
         <v>635</v>
@@ -9732,27 +9790,30 @@
         <v>518</v>
       </c>
       <c r="J120">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>523</v>
+        <v>651</v>
       </c>
       <c r="L120" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B121" t="s">
-        <v>531</v>
+        <v>526</v>
+      </c>
+      <c r="C121" t="s">
+        <v>688</v>
       </c>
       <c r="D121" t="s">
         <v>635</v>
       </c>
       <c r="E121" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
       <c r="F121" t="s">
         <v>647</v>
@@ -9761,27 +9822,27 @@
         <v>641</v>
       </c>
       <c r="H121" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I121" t="s">
         <v>518</v>
       </c>
       <c r="J121">
-        <v>368</v>
+        <v>5</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>523</v>
+        <v>649</v>
       </c>
       <c r="L121" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B122" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D122" t="s">
         <v>635</v>
@@ -9796,27 +9857,27 @@
         <v>641</v>
       </c>
       <c r="H122" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I122" t="s">
         <v>518</v>
       </c>
       <c r="J122">
-        <v>368</v>
+        <v>11</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>523</v>
+        <v>650</v>
       </c>
       <c r="L122" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B123" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D123" t="s">
         <v>635</v>
@@ -9831,30 +9892,33 @@
         <v>641</v>
       </c>
       <c r="H123" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I123" t="s">
         <v>518</v>
       </c>
       <c r="J123">
-        <v>368</v>
+        <v>4</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>523</v>
+        <v>651</v>
       </c>
       <c r="L123" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B124" t="s">
-        <v>250</v>
+        <v>529</v>
       </c>
       <c r="D124" t="s">
         <v>635</v>
+      </c>
+      <c r="E124" t="s">
+        <v>638</v>
       </c>
       <c r="F124" t="s">
         <v>647</v>
@@ -9869,36 +9933,33 @@
         <v>518</v>
       </c>
       <c r="J124">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>339</v>
+        <v>523</v>
       </c>
       <c r="L124" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B125" t="s">
-        <v>251</v>
-      </c>
-      <c r="C125" t="s">
-        <v>680</v>
+        <v>530</v>
       </c>
       <c r="D125" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="E125" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F125" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="G125" t="s">
-        <v>653</v>
+        <v>641</v>
       </c>
       <c r="H125" t="s">
         <v>6</v>
@@ -9907,24 +9968,21 @@
         <v>518</v>
       </c>
       <c r="J125">
-        <v>714167</v>
+        <v>2</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>260</v>
+        <v>523</v>
       </c>
       <c r="L125" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B126" t="s">
-        <v>254</v>
-      </c>
-      <c r="C126" t="s">
-        <v>681</v>
+        <v>531</v>
       </c>
       <c r="D126" t="s">
         <v>635</v>
@@ -9933,24 +9991,202 @@
         <v>638</v>
       </c>
       <c r="F126" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="G126" t="s">
         <v>641</v>
       </c>
       <c r="H126" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I126" t="s">
         <v>518</v>
       </c>
       <c r="J126">
+        <v>368</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="L126" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>121</v>
+      </c>
+      <c r="B127" t="s">
+        <v>532</v>
+      </c>
+      <c r="D127" t="s">
+        <v>635</v>
+      </c>
+      <c r="E127" t="s">
+        <v>638</v>
+      </c>
+      <c r="F127" t="s">
+        <v>647</v>
+      </c>
+      <c r="G127" t="s">
+        <v>641</v>
+      </c>
+      <c r="H127" t="s">
+        <v>1</v>
+      </c>
+      <c r="I127" t="s">
+        <v>518</v>
+      </c>
+      <c r="J127">
+        <v>368</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="L127" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>122</v>
+      </c>
+      <c r="B128" t="s">
+        <v>533</v>
+      </c>
+      <c r="D128" t="s">
+        <v>635</v>
+      </c>
+      <c r="E128" t="s">
+        <v>638</v>
+      </c>
+      <c r="F128" t="s">
+        <v>647</v>
+      </c>
+      <c r="G128" t="s">
+        <v>641</v>
+      </c>
+      <c r="H128" t="s">
+        <v>1</v>
+      </c>
+      <c r="I128" t="s">
+        <v>518</v>
+      </c>
+      <c r="J128">
+        <v>368</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="L128" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" ht="28.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>123</v>
+      </c>
+      <c r="B129" t="s">
+        <v>250</v>
+      </c>
+      <c r="D129" t="s">
+        <v>635</v>
+      </c>
+      <c r="F129" t="s">
+        <v>647</v>
+      </c>
+      <c r="G129" t="s">
+        <v>641</v>
+      </c>
+      <c r="H129" t="s">
+        <v>6</v>
+      </c>
+      <c r="I129" t="s">
+        <v>518</v>
+      </c>
+      <c r="J129">
+        <v>3</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="L129" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>124</v>
+      </c>
+      <c r="B130" t="s">
+        <v>251</v>
+      </c>
+      <c r="C130" t="s">
+        <v>679</v>
+      </c>
+      <c r="D130" t="s">
+        <v>634</v>
+      </c>
+      <c r="E130" t="s">
+        <v>637</v>
+      </c>
+      <c r="F130" t="s">
+        <v>646</v>
+      </c>
+      <c r="G130" t="s">
+        <v>653</v>
+      </c>
+      <c r="H130" t="s">
+        <v>6</v>
+      </c>
+      <c r="I130" t="s">
+        <v>518</v>
+      </c>
+      <c r="J130">
+        <v>714167</v>
+      </c>
+      <c r="K130" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="L130" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>125</v>
+      </c>
+      <c r="B131" t="s">
+        <v>254</v>
+      </c>
+      <c r="C131" t="s">
+        <v>680</v>
+      </c>
+      <c r="D131" t="s">
+        <v>635</v>
+      </c>
+      <c r="E131" t="s">
+        <v>638</v>
+      </c>
+      <c r="F131" t="s">
+        <v>646</v>
+      </c>
+      <c r="G131" t="s">
+        <v>641</v>
+      </c>
+      <c r="H131" t="s">
+        <v>6</v>
+      </c>
+      <c r="I131" t="s">
+        <v>518</v>
+      </c>
+      <c r="J131">
         <v>8</v>
       </c>
-      <c r="K126" s="1" t="s">
+      <c r="K131" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="L126" t="s">
+      <c r="L131" t="s">
         <v>630</v>
       </c>
     </row>

</xml_diff>